<commit_message>
Completed till checkpoint 3
</commit_message>
<xml_diff>
--- a/InvestmentAnalysis/results/Investments.xlsx
+++ b/InvestmentAnalysis/results/Investments.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Investment case study Cohort-3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
   </bookViews>
@@ -17,23 +12,12 @@
     <sheet name="Table-3.1" sheetId="5" r:id="rId3"/>
     <sheet name="Table-5.1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>C1</t>
   </si>
@@ -357,12 +341,30 @@
   </si>
   <si>
     <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Venture Type</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,24 +634,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -665,27 +670,49 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -734,7 +761,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -786,7 +813,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -980,7 +1007,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -991,7 +1018,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,23 +1029,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1038,7 +1065,9 @@
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>66102</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1047,7 +1076,9 @@
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="17">
+        <v>66368</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -1056,7 +1087,9 @@
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1065,7 +1098,9 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1074,7 +1109,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17">
+        <v>114949</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
@@ -1098,6 +1135,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1106,7 +1144,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,21 +1155,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1151,7 +1189,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>11748950</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1160,7 +1200,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>958694.5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -1169,7 +1211,9 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>719818</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1178,7 +1222,9 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <v>73308590</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1187,7 +1233,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1214,7 +1262,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,21 +1273,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1259,7 +1307,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1268,7 +1318,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1277,7 +1329,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1303,7 +1357,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,38 +1370,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>